<commit_message>
ggh summary table update
</commit_message>
<xml_diff>
--- a/ggh-growth/ggh-growth-summary.xlsx
+++ b/ggh-growth/ggh-growth-summary.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Population &amp; Households by Regi" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Dwelling Types" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Growth Population &amp; Households " sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Growth by Dwelling Types" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
   <si>
     <t xml:space="preserve">Population</t>
   </si>
@@ -71,9 +71,6 @@
     <t xml:space="preserve">GTHA SubTotal</t>
   </si>
   <si>
-    <t xml:space="preserve">Total Inner Ring</t>
-  </si>
-  <si>
     <t xml:space="preserve">Outer Ring</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
   </si>
   <si>
     <t xml:space="preserve">Outer Ring SubTotal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Outer Ring</t>
   </si>
   <si>
     <t xml:space="preserve">Grand Total</t>
@@ -492,11 +486,11 @@
   </sheetPr>
   <dimension ref="B1:AMJ26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.93"/>
@@ -768,9 +762,7 @@
       <c r="B10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>16</v>
-      </c>
+      <c r="C10" s="19"/>
       <c r="D10" s="20" t="n">
         <v>1235132</v>
       </c>
@@ -798,10 +790,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>14496</v>
@@ -830,10 +822,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>28797</v>
@@ -862,10 +854,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>4686</v>
@@ -894,10 +886,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>3466</v>
@@ -926,10 +918,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>8753</v>
@@ -958,10 +950,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>5059</v>
@@ -990,10 +982,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>11821</v>
@@ -1022,10 +1014,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>4004</v>
@@ -1054,10 +1046,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>8564</v>
@@ -1086,10 +1078,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>6331</v>
@@ -1118,10 +1110,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="15" t="n">
         <v>89420</v>
@@ -1150,10 +1142,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="15" t="n">
         <v>11804</v>
@@ -1182,10 +1174,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="15" t="n">
         <v>50520</v>
@@ -1214,10 +1206,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" s="15" t="n">
         <v>110614</v>
@@ -1246,11 +1238,9 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>33</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C25" s="19"/>
       <c r="D25" s="20" t="n">
         <v>378391</v>
       </c>
@@ -1278,10 +1268,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D26" s="25" t="n">
         <v>1613523</v>
@@ -1330,11 +1320,11 @@
   </sheetPr>
   <dimension ref="B1:J23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.65"/>
@@ -1355,12 +1345,12 @@
         <v>6</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="29" t="n">
         <v>689015</v>
@@ -1377,7 +1367,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>252745</v>
@@ -1394,7 +1384,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>32040</v>
@@ -1411,7 +1401,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>103205</v>
@@ -1428,7 +1418,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>17960</v>
@@ -1445,7 +1435,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>33860</v>
@@ -1462,7 +1452,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>243780</v>
@@ -1479,7 +1469,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,28 +1477,28 @@
         <v>4</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="G14" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="I14" s="30" t="s">
         <v>48</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="I14" s="30" t="s">
-        <v>50</v>
       </c>
       <c r="J14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="31" t="n">
         <v>689015</v>
@@ -1540,7 +1530,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16" s="33" t="n">
         <v>1</v>
@@ -1563,7 +1553,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17" s="34" t="n">
         <f aca="false">(C3*D3/100) / D$15</f>
@@ -1592,7 +1582,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" s="34" t="n">
         <f aca="false">(C4*D4/100) / D$15</f>
@@ -1621,7 +1611,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="34" t="n">
         <f aca="false">(C5*D5/100) / D$15</f>
@@ -1650,7 +1640,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20" s="34" t="n">
         <f aca="false">(C6*D6/100) / D$15</f>
@@ -1679,7 +1669,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" s="34" t="n">
         <f aca="false">(C7*D7/100) / D$15</f>
@@ -1708,7 +1698,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D22" s="34" t="n">
         <f aca="false">(C8*D8/100) / D$15</f>
@@ -1737,7 +1727,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D23" s="33" t="n">
         <f aca="false">D16-SUM(D17:D22)</f>

</xml_diff>